<commit_message>
fit indices and cleaned-up figures
</commit_message>
<xml_diff>
--- a/modification indices KEY.xlsx
+++ b/modification indices KEY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kulas\Git\SIOP-Engagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC25D69-BB45-4496-9D64-30F48911CE3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4927C9A-8485-4D72-B20F-B570D14EC0B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16500" yWindow="1860" windowWidth="12960" windowHeight="8040" firstSheet="2" activeTab="3" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
+    <workbookView xWindow="16500" yWindow="1860" windowWidth="12960" windowHeight="8040" firstSheet="2" activeTab="5" xr2:uid="{B771755A-0338-4D98-8477-C34FFA1BF3E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="89">
   <si>
     <t>item</t>
   </si>
@@ -310,6 +310,27 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>Item_1=I am able to concentrate on my work without getting distracted</t>
+  </si>
+  <si>
+    <t>Final Construct Validation Set</t>
+  </si>
+  <si>
+    <t>Item_25=I plan to stay with this company as my career advances</t>
+  </si>
+  <si>
+    <t>Item_19=I feel motivated to go beyond what is asked of me at work</t>
+  </si>
+  <si>
+    <t>1,3,4,14,16,25,26,28</t>
+  </si>
+  <si>
+    <t>5,8,17,19,31,32</t>
+  </si>
+  <si>
+    <t>10,11,21,22,34,35</t>
   </si>
 </sst>
 </file>
@@ -2697,7 +2718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42093553-B6C7-40A0-B0F3-9D76C93911BE}">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -4085,19 +4106,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222B1B82-4AC1-4BFA-9AA2-5AB35BC453AE}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="81.44140625" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="11" max="11" width="78.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -4107,8 +4129,11 @@
       <c r="C1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>32</v>
       </c>
@@ -4116,8 +4141,11 @@
       <c r="C2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="K2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>77</v>
       </c>
@@ -4125,56 +4153,83 @@
       <c r="C3" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="K3" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="K4" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="7"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="K5" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B6" s="7"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="K6" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="22"/>
-    </row>
-    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="K7" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="28" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="22"/>
-    </row>
-    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="K8" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
         <v>45</v>
       </c>
       <c r="B9" s="15"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="K9" s="25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="15"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="K10" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>48</v>
       </c>
       <c r="B11" s="27"/>
-    </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="K11" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
         <v>74</v>
       </c>
@@ -4182,32 +4237,47 @@
       <c r="C12" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="K12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="28" t="s">
         <v>52</v>
       </c>
       <c r="B13" s="22"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="K13" s="28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>53</v>
       </c>
       <c r="B14" s="22"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="K14" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>57</v>
       </c>
       <c r="B15" s="15"/>
-    </row>
-    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="K15" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="25" t="s">
         <v>59</v>
       </c>
       <c r="B16" s="15"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="K16" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>56</v>
       </c>
@@ -4215,30 +4285,60 @@
       <c r="C17" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="K17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>62</v>
       </c>
       <c r="B18" s="27"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="K18" s="27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>63</v>
       </c>
       <c r="B19" s="27"/>
-    </row>
-    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="K19" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="28" t="s">
         <v>65</v>
       </c>
       <c r="B20" s="22"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="K20" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
         <v>66</v>
       </c>
       <c r="B21" s="22"/>
+      <c r="K21" s="22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K26" t="s">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>